<commit_message>
Added documentation for array function
</commit_message>
<xml_diff>
--- a/doc/commands.xlsx
+++ b/doc/commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gtggbg-my.sharepoint.com/personal/oscar_melander_gtg-educ_com/Documents/GTG/Te3c/Examensarbete/GICU-3/GICU-3-Server/GICU-3-Server/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="11_F25DC773A252ABDACC104892695B6CCE5BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC28707F-6B77-4A0B-A799-D0B5BBD1B89C}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="11_F25DC773A252ABDACC104892695B6CCE5BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F18CE10-D6FF-44AD-990E-DC2DE5ADF505}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-2820" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Commands</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>Restarts server</t>
+  </si>
+  <si>
+    <t>array([n,m,o],color)</t>
+  </si>
+  <si>
+    <t>array([2,6,9],0xFFFFFF)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sets multiple pixels in array a certain color </t>
   </si>
 </sst>
 </file>
@@ -227,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -249,6 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,43 +614,49 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
+      <c r="A7" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
     </row>
@@ -664,12 +680,18 @@
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C16"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>